<commit_message>
Removing temporaty data and heavy files, and minor changes
</commit_message>
<xml_diff>
--- a/Results/Sodx_Unstructured/Case Guide.xlsx
+++ b/Results/Sodx_Unstructured/Case Guide.xlsx
@@ -330,10 +330,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.086109895605426"/>
+          <c:x val="0.0860786397449522"/>
           <c:y val="0.0347893742358564"/>
-          <c:w val="0.688066512471088"/>
-          <c:h val="0.865844170278982"/>
+          <c:w val="0.688004000750141"/>
+          <c:h val="0.865733022118484"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -416,7 +416,7 @@
                   <c:v>0.00390625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.001953125</c:v>
+                  <c:v>0.0625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,18 +449,18 @@
                   <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1024</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42008010"/>
-        <c:axId val="11877594"/>
+        <c:axId val="62106433"/>
+        <c:axId val="35940555"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42008010"/>
+        <c:axId val="62106433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,12 +488,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11877594"/>
+        <c:crossAx val="35940555"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11877594"/>
+        <c:axId val="35940555"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +530,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42008010"/>
+        <c:crossAx val="62106433"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -589,9 +589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>574200</xdr:colOff>
+      <xdr:colOff>573840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -600,7 +600,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1317600" y="1677960"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -618,15 +618,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,6 +750,7 @@
         <f aca="false">2/C7</f>
         <v>0.03125</v>
       </c>
+      <c r="M7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="n">
@@ -769,6 +772,7 @@
         <f aca="false">2/C8</f>
         <v>0.0078125</v>
       </c>
+      <c r="M8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
@@ -796,20 +800,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="n">
-        <f aca="false">C9*2</f>
-        <v>1024</v>
+        <f aca="false">C7/2</f>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="n">
-        <f aca="false">D9*2</f>
-        <v>1024</v>
+        <v>32</v>
       </c>
       <c r="E10" s="12" t="n">
         <f aca="false">D10*C10</f>
-        <v>1048576</v>
+        <v>1024</v>
       </c>
       <c r="F10" s="6" t="n">
         <f aca="false">2/C10</f>
-        <v>0.001953125</v>
+        <v>0.0625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>